<commit_message>
Pivot Table is added
</commit_message>
<xml_diff>
--- a/day5_Personal_Monthly_Expenditure.xlsx
+++ b/day5_Personal_Monthly_Expenditure.xlsx
@@ -1,21 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Excel-For-Data-Analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{81246ABE-1E35-44C1-BF61-287236215A4E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EB131AD-987F-49CE-81AA-D3C02AE995DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Expense - 2018" sheetId="1" r:id="rId1"/>
+    <sheet name="Pivot Table" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191028"/>
+  <pivotCaches>
+    <pivotCache cacheId="3" r:id="rId3"/>
+  </pivotCaches>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -30,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="29">
   <si>
     <t>Month</t>
   </si>
@@ -109,13 +113,22 @@
   <si>
     <t>MEDIAN</t>
   </si>
+  <si>
+    <t>Row Labels</t>
+  </si>
+  <si>
+    <t>Grand Total</t>
+  </si>
+  <si>
+    <t>Sum of Monthly Total</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="&quot;₹&quot;\ #,##0.00"/>
+    <numFmt numFmtId="164" formatCode="&quot;₹&quot;\ #,##0.00"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -161,17 +174,63 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="34">
+    <dxf>
+      <numFmt numFmtId="164" formatCode="&quot;₹&quot;\ #,##0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="&quot;₹&quot;\ #,##0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="&quot;₹&quot;\ #,##0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="&quot;₹&quot;\ #,##0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="&quot;₹&quot;\ #,##0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="&quot;₹&quot;\ #,##0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="&quot;₹&quot;\ #,##0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="&quot;₹&quot;\ #,##0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="&quot;₹&quot;\ #,##0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="&quot;₹&quot;\ #,##0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="&quot;₹&quot;\ #,##0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="&quot;₹&quot;\ #,##0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="&quot;₹&quot;\ #,##0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="&quot;₹&quot;\ #,##0.00"/>
+    </dxf>
     <dxf>
       <font>
         <b/>
@@ -191,51 +250,6 @@
       </font>
     </dxf>
     <dxf>
-      <numFmt numFmtId="165" formatCode="&quot;₹&quot;\ #,##0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="&quot;₹&quot;\ #,##0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="&quot;₹&quot;\ #,##0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="&quot;₹&quot;\ #,##0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="&quot;₹&quot;\ #,##0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="&quot;₹&quot;\ #,##0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="&quot;₹&quot;\ #,##0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="&quot;₹&quot;\ #,##0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="&quot;₹&quot;\ #,##0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="&quot;₹&quot;\ #,##0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="&quot;₹&quot;\ #,##0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="&quot;₹&quot;\ #,##0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="&quot;₹&quot;\ #,##0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="&quot;₹&quot;\ #,##0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="&quot;₹&quot;\ #,##0.00"/>
-    </dxf>
-    <dxf>
       <font>
         <b/>
         <i val="0"/>
@@ -254,31 +268,7 @@
       </font>
     </dxf>
     <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="165" formatCode="&quot;₹&quot;\ #,##0.00"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <protection locked="1" hidden="0"/>
+      <numFmt numFmtId="164" formatCode="&quot;₹&quot;\ #,##0.00"/>
     </dxf>
     <dxf>
       <font>
@@ -323,168 +313,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
-      <numFmt numFmtId="165" formatCode="&quot;₹&quot;\ #,##0.00"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <protection locked="1" hidden="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="165" formatCode="&quot;₹&quot;\ #,##0.00"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <protection locked="1" hidden="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="165" formatCode="&quot;₹&quot;\ #,##0.00"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <protection locked="1" hidden="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="165" formatCode="&quot;₹&quot;\ #,##0.00"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <protection locked="1" hidden="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="165" formatCode="&quot;₹&quot;\ #,##0.00"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <protection locked="1" hidden="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="165" formatCode="&quot;₹&quot;\ #,##0.00"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <protection locked="1" hidden="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
+      <numFmt numFmtId="164" formatCode="&quot;₹&quot;\ #,##0.00"/>
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
@@ -537,7 +366,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
-      <numFmt numFmtId="164" formatCode="_-[$£-809]* #,##0.00_-;\-[$£-809]* #,##0.00_-;_-[$£-809]* &quot;-&quot;??_-;_-@_-"/>
+      <numFmt numFmtId="164" formatCode="&quot;₹&quot;\ #,##0.00"/>
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
@@ -564,7 +393,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
-      <numFmt numFmtId="164" formatCode="_-[$£-809]* #,##0.00_-;\-[$£-809]* #,##0.00_-;_-[$£-809]* &quot;-&quot;??_-;_-@_-"/>
+      <numFmt numFmtId="165" formatCode="_-[$£-809]* #,##0.00_-;\-[$£-809]* #,##0.00_-;_-[$£-809]* &quot;-&quot;??_-;_-@_-"/>
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
@@ -591,7 +420,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
-      <numFmt numFmtId="164" formatCode="_-[$£-809]* #,##0.00_-;\-[$£-809]* #,##0.00_-;_-[$£-809]* &quot;-&quot;??_-;_-@_-"/>
+      <numFmt numFmtId="164" formatCode="&quot;₹&quot;\ #,##0.00"/>
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
@@ -618,7 +447,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
-      <numFmt numFmtId="164" formatCode="_-[$£-809]* #,##0.00_-;\-[$£-809]* #,##0.00_-;_-[$£-809]* &quot;-&quot;??_-;_-@_-"/>
+      <numFmt numFmtId="165" formatCode="_-[$£-809]* #,##0.00_-;\-[$£-809]* #,##0.00_-;_-[$£-809]* &quot;-&quot;??_-;_-@_-"/>
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
@@ -645,7 +474,195 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
-      <numFmt numFmtId="164" formatCode="_-[$£-809]* #,##0.00_-;\-[$£-809]* #,##0.00_-;_-[$£-809]* &quot;-&quot;??_-;_-@_-"/>
+      <numFmt numFmtId="164" formatCode="&quot;₹&quot;\ #,##0.00"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="165" formatCode="_-[$£-809]* #,##0.00_-;\-[$£-809]* #,##0.00_-;_-[$£-809]* &quot;-&quot;??_-;_-@_-"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="164" formatCode="&quot;₹&quot;\ #,##0.00"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="165" formatCode="_-[$£-809]* #,##0.00_-;\-[$£-809]* #,##0.00_-;_-[$£-809]* &quot;-&quot;??_-;_-@_-"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="164" formatCode="&quot;₹&quot;\ #,##0.00"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="165" formatCode="_-[$£-809]* #,##0.00_-;\-[$£-809]* #,##0.00_-;_-[$£-809]* &quot;-&quot;??_-;_-@_-"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="164" formatCode="&quot;₹&quot;\ #,##0.00"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
@@ -722,18 +739,1433 @@
 </styleSheet>
 </file>
 
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:pivotSource>
+    <c:name>[day5_Personal_Monthly_Expenditure.xlsx]Pivot Table!PivotTable1</c:name>
+    <c:fmtId val="0"/>
+  </c:pivotSource>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:pivotFmts>
+      <c:pivotFmt>
+        <c:idx val="0"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln w="19050">
+            <a:solidFill>
+              <a:schemeClr val="lt1"/>
+            </a:solidFill>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+        <c:dLbl>
+          <c:idx val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="75000"/>
+                      <a:lumOff val="25000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+          </c:extLst>
+        </c:dLbl>
+      </c:pivotFmt>
+    </c:pivotFmts>
+    <c:plotArea>
+      <c:layout/>
+      <c:pieChart>
+        <c:varyColors val="1"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Pivot Table'!$B$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Total</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="2"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="3"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="4"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="5"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="6"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="7"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="8"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="9"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="10"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent5">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="11"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent6">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Pivot Table'!$A$4:$A$16</c:f>
+              <c:strCache>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>Dec</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Nov</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Oct</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Sep</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Aug</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Jul</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Jun</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>May</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Apr</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Mar</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>Feb</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>Jan</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Pivot Table'!$B$4:$B$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>1695</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1660</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1650</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1640</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1650</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1650</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1620</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1650</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1640</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1670</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1625</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1670</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-5320-48A8-8D15-959AA7EB24AE}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:showLeaderLines val="1"/>
+        </c:dLbls>
+        <c:firstSliceAng val="0"/>
+      </c:pieChart>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+  <c:extLst>
+    <c:ext xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" uri="{781A3756-C4B2-4CAC-9D66-4F8BD8637D16}">
+      <c14:pivotOptions>
+        <c14:dropZoneFilter val="1"/>
+        <c14:dropZoneCategories val="1"/>
+        <c14:dropZoneData val="1"/>
+        <c14:dropZoneSeries val="1"/>
+        <c14:dropZonesVisible val="1"/>
+      </c14:pivotOptions>
+    </c:ext>
+    <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{E28EC0CA-F0BB-4C9C-879D-F8772B89E7AC}">
+      <c16:pivotOptions16>
+        <c16:showExpandCollapseFieldButtons val="1"/>
+      </c16:pivotOptions16>
+    </c:ext>
+  </c:extLst>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="251">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="25400">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>1257300</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>228600</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9EDD0CFB-A15A-C7E0-2980-F73A47603A1E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Obito Uchiha" refreshedDate="45458.954999189817" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="13" xr:uid="{945F9F18-2EFB-46F9-99AF-66B668E90E89}">
+  <cacheSource type="worksheet">
+    <worksheetSource ref="A1:H14" sheet="Expense - 2018"/>
+  </cacheSource>
+  <cacheFields count="8">
+    <cacheField name="Month" numFmtId="0">
+      <sharedItems containsBlank="1" count="13">
+        <s v="Jan"/>
+        <s v="Feb"/>
+        <s v="Mar"/>
+        <s v="Apr"/>
+        <s v="May"/>
+        <s v="Jun"/>
+        <s v="Jul"/>
+        <s v="Aug"/>
+        <s v="Sep"/>
+        <s v="Oct"/>
+        <s v="Nov"/>
+        <s v="Dec"/>
+        <m/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="Housing" numFmtId="164">
+      <sharedItems containsString="0" containsBlank="1" containsNumber="1" containsInteger="1" minValue="800" maxValue="800"/>
+    </cacheField>
+    <cacheField name="Bills &amp; Utilities" numFmtId="164">
+      <sharedItems containsString="0" containsBlank="1" containsNumber="1" containsInteger="1" minValue="150" maxValue="220"/>
+    </cacheField>
+    <cacheField name="Food &amp; Dining" numFmtId="164">
+      <sharedItems containsString="0" containsBlank="1" containsNumber="1" containsInteger="1" minValue="350" maxValue="420"/>
+    </cacheField>
+    <cacheField name="Personal" numFmtId="164">
+      <sharedItems containsString="0" containsBlank="1" containsNumber="1" containsInteger="1" minValue="100" maxValue="120"/>
+    </cacheField>
+    <cacheField name="Auto &amp; Transport" numFmtId="164">
+      <sharedItems containsString="0" containsBlank="1" containsNumber="1" containsInteger="1" minValue="100" maxValue="130"/>
+    </cacheField>
+    <cacheField name="Health &amp; Fitness" numFmtId="164">
+      <sharedItems containsString="0" containsBlank="1" containsNumber="1" containsInteger="1" minValue="50" maxValue="80"/>
+    </cacheField>
+    <cacheField name="Monthly Total" numFmtId="164">
+      <sharedItems containsString="0" containsBlank="1" containsNumber="1" containsInteger="1" minValue="1620" maxValue="1695"/>
+    </cacheField>
+  </cacheFields>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{725AE2AE-9491-48be-B2B4-4EB974FC3084}">
+      <x14:pivotCacheDefinition/>
+    </ext>
+  </extLst>
+</pivotCacheDefinition>
+</file>
+
+<file path=xl/pivotCache/pivotCacheRecords1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" count="13">
+  <r>
+    <x v="0"/>
+    <n v="800"/>
+    <n v="210"/>
+    <n v="400"/>
+    <n v="100"/>
+    <n v="100"/>
+    <n v="60"/>
+    <n v="1670"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <n v="800"/>
+    <n v="180"/>
+    <n v="350"/>
+    <n v="100"/>
+    <n v="125"/>
+    <n v="70"/>
+    <n v="1625"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <n v="800"/>
+    <n v="170"/>
+    <n v="420"/>
+    <n v="100"/>
+    <n v="120"/>
+    <n v="60"/>
+    <n v="1670"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <n v="800"/>
+    <n v="160"/>
+    <n v="400"/>
+    <n v="120"/>
+    <n v="100"/>
+    <n v="60"/>
+    <n v="1640"/>
+  </r>
+  <r>
+    <x v="4"/>
+    <n v="800"/>
+    <n v="150"/>
+    <n v="420"/>
+    <n v="100"/>
+    <n v="100"/>
+    <n v="80"/>
+    <n v="1650"/>
+  </r>
+  <r>
+    <x v="5"/>
+    <n v="800"/>
+    <n v="150"/>
+    <n v="380"/>
+    <n v="100"/>
+    <n v="130"/>
+    <n v="60"/>
+    <n v="1620"/>
+  </r>
+  <r>
+    <x v="6"/>
+    <n v="800"/>
+    <n v="150"/>
+    <n v="420"/>
+    <n v="120"/>
+    <n v="100"/>
+    <n v="60"/>
+    <n v="1650"/>
+  </r>
+  <r>
+    <x v="7"/>
+    <n v="800"/>
+    <n v="150"/>
+    <n v="420"/>
+    <n v="100"/>
+    <n v="100"/>
+    <n v="80"/>
+    <n v="1650"/>
+  </r>
+  <r>
+    <x v="8"/>
+    <n v="800"/>
+    <n v="150"/>
+    <n v="400"/>
+    <n v="120"/>
+    <n v="110"/>
+    <n v="60"/>
+    <n v="1640"/>
+  </r>
+  <r>
+    <x v="9"/>
+    <n v="800"/>
+    <n v="170"/>
+    <n v="420"/>
+    <n v="100"/>
+    <n v="100"/>
+    <n v="60"/>
+    <n v="1650"/>
+  </r>
+  <r>
+    <x v="10"/>
+    <n v="800"/>
+    <n v="200"/>
+    <n v="390"/>
+    <n v="120"/>
+    <n v="100"/>
+    <n v="50"/>
+    <n v="1660"/>
+  </r>
+  <r>
+    <x v="11"/>
+    <n v="800"/>
+    <n v="220"/>
+    <n v="400"/>
+    <n v="100"/>
+    <n v="115"/>
+    <n v="60"/>
+    <n v="1695"/>
+  </r>
+  <r>
+    <x v="12"/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+  </r>
+</pivotCacheRecords>
+</file>
+
+<file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{12716CCC-BE3A-4985-9150-3CBAAA8B49B9}" name="PivotTable1" cacheId="3" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
+  <location ref="A3:B16" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="8">
+    <pivotField axis="axisRow" showAll="0" sortType="descending">
+      <items count="14">
+        <item h="1" x="12"/>
+        <item x="11"/>
+        <item x="10"/>
+        <item x="9"/>
+        <item x="8"/>
+        <item x="7"/>
+        <item x="6"/>
+        <item x="5"/>
+        <item x="4"/>
+        <item x="3"/>
+        <item x="2"/>
+        <item x="1"/>
+        <item x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField dataField="1" showAll="0"/>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="0"/>
+  </rowFields>
+  <rowItems count="13">
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="4"/>
+    </i>
+    <i>
+      <x v="5"/>
+    </i>
+    <i>
+      <x v="6"/>
+    </i>
+    <i>
+      <x v="7"/>
+    </i>
+    <i>
+      <x v="8"/>
+    </i>
+    <i>
+      <x v="9"/>
+    </i>
+    <i>
+      <x v="10"/>
+    </i>
+    <i>
+      <x v="11"/>
+    </i>
+    <i>
+      <x v="12"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Sum of Monthly Total" fld="7" baseField="0" baseItem="0"/>
+  </dataFields>
+  <chartFormats count="1">
+    <chartFormat chart="0" format="0" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+  </chartFormats>
+  <pivotTableStyleInfo name="PivotStyleMedium9" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{AB075690-6493-4B96-8D1B-B29AB2D9E9A9}" name="Table6" displayName="Table6" ref="A1:H13" totalsRowShown="0" headerRowDxfId="33" dataDxfId="32">
   <autoFilter ref="A1:H13" xr:uid="{1C96BD00-98D9-4572-8F4A-F406BBA95AE3}"/>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{0738465F-87B9-46AD-8314-585AF20E321C}" name="Month" dataDxfId="25"/>
-    <tableColumn id="2" xr3:uid="{639B5A90-C646-4312-A12B-90EBA415C5F3}" name="Housing" dataDxfId="24" totalsRowDxfId="31"/>
-    <tableColumn id="3" xr3:uid="{AC863E34-6694-4292-A7E8-5D94B1D4B90E}" name="Bills &amp; Utilities" dataDxfId="23" totalsRowDxfId="30"/>
-    <tableColumn id="4" xr3:uid="{7F96B093-000D-47C8-9B3D-9C6DC794A7DD}" name="Food &amp; Dining" dataDxfId="22" totalsRowDxfId="29"/>
-    <tableColumn id="5" xr3:uid="{0D73BCA8-FF88-432A-8438-8D3C42615074}" name="Personal" dataDxfId="21" totalsRowDxfId="28"/>
-    <tableColumn id="6" xr3:uid="{62ECB4B2-7FAC-4168-96E6-6A3296B9F2CB}" name="Auto &amp; Transport" dataDxfId="20" totalsRowDxfId="27"/>
-    <tableColumn id="7" xr3:uid="{5C8E2143-EA5D-49A7-8A33-6E4F45D73494}" name="Health &amp; Fitness" dataDxfId="19" totalsRowDxfId="26"/>
-    <tableColumn id="8" xr3:uid="{E91C1945-9F36-4DF8-9C0A-34FDC1B298E9}" name="Monthly Total" dataDxfId="17" totalsRowDxfId="18">
+    <tableColumn id="1" xr3:uid="{0738465F-87B9-46AD-8314-585AF20E321C}" name="Month" dataDxfId="31"/>
+    <tableColumn id="2" xr3:uid="{639B5A90-C646-4312-A12B-90EBA415C5F3}" name="Housing" dataDxfId="30" totalsRowDxfId="29"/>
+    <tableColumn id="3" xr3:uid="{AC863E34-6694-4292-A7E8-5D94B1D4B90E}" name="Bills &amp; Utilities" dataDxfId="28" totalsRowDxfId="27"/>
+    <tableColumn id="4" xr3:uid="{7F96B093-000D-47C8-9B3D-9C6DC794A7DD}" name="Food &amp; Dining" dataDxfId="26" totalsRowDxfId="25"/>
+    <tableColumn id="5" xr3:uid="{0D73BCA8-FF88-432A-8438-8D3C42615074}" name="Personal" dataDxfId="24" totalsRowDxfId="23"/>
+    <tableColumn id="6" xr3:uid="{62ECB4B2-7FAC-4168-96E6-6A3296B9F2CB}" name="Auto &amp; Transport" dataDxfId="22" totalsRowDxfId="21"/>
+    <tableColumn id="7" xr3:uid="{5C8E2143-EA5D-49A7-8A33-6E4F45D73494}" name="Health &amp; Fitness" dataDxfId="20" totalsRowDxfId="19"/>
+    <tableColumn id="8" xr3:uid="{E91C1945-9F36-4DF8-9C0A-34FDC1B298E9}" name="Monthly Total" dataDxfId="18" totalsRowDxfId="17">
       <calculatedColumnFormula>SUM(Table6[[#This Row],[Housing]:[Health &amp; Fitness]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -742,16 +2174,16 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{1D3A6644-50C0-46C4-875C-D6410981351D}" name="Table1" displayName="Table1" ref="A16:H22" headerRowCount="0" totalsRowShown="0" headerRowDxfId="8">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{1D3A6644-50C0-46C4-875C-D6410981351D}" name="Table1" displayName="Table1" ref="A16:H22" headerRowCount="0" totalsRowShown="0" headerRowDxfId="16">
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{76091C81-913D-476F-A20D-F273AA405232}" name="Column1" headerRowDxfId="0" dataDxfId="16"/>
-    <tableColumn id="2" xr3:uid="{D9A27D4A-3D46-4837-A3D8-3D0A5F3F327D}" name="Column2" headerRowDxfId="1" dataDxfId="15"/>
-    <tableColumn id="3" xr3:uid="{076A42E2-9A2E-4F82-B482-13E888FA5CC8}" name="Column3" headerRowDxfId="2" dataDxfId="14"/>
-    <tableColumn id="4" xr3:uid="{E0B23A7F-19D4-4E3B-8CBE-B48CDBC9C573}" name="Column4" headerRowDxfId="3" dataDxfId="13"/>
-    <tableColumn id="5" xr3:uid="{223CB90B-F16D-41E5-B97B-E4014F67D120}" name="Column5" headerRowDxfId="4" dataDxfId="12"/>
-    <tableColumn id="6" xr3:uid="{BF227374-82A0-4088-A70D-4967E9D58339}" name="Column6" headerRowDxfId="5" dataDxfId="11"/>
-    <tableColumn id="7" xr3:uid="{BA7D3376-9D4B-4B12-AB45-3526E423DA24}" name="Column7" headerRowDxfId="6" dataDxfId="10"/>
-    <tableColumn id="8" xr3:uid="{B23F41D5-4E64-4061-94AA-F7D64566A5B8}" name="Column8" headerRowDxfId="7" dataDxfId="9"/>
+    <tableColumn id="1" xr3:uid="{76091C81-913D-476F-A20D-F273AA405232}" name="Column1" headerRowDxfId="15" dataDxfId="14"/>
+    <tableColumn id="2" xr3:uid="{D9A27D4A-3D46-4837-A3D8-3D0A5F3F327D}" name="Column2" headerRowDxfId="13" dataDxfId="12"/>
+    <tableColumn id="3" xr3:uid="{076A42E2-9A2E-4F82-B482-13E888FA5CC8}" name="Column3" headerRowDxfId="11" dataDxfId="10"/>
+    <tableColumn id="4" xr3:uid="{E0B23A7F-19D4-4E3B-8CBE-B48CDBC9C573}" name="Column4" headerRowDxfId="9" dataDxfId="8"/>
+    <tableColumn id="5" xr3:uid="{223CB90B-F16D-41E5-B97B-E4014F67D120}" name="Column5" headerRowDxfId="7" dataDxfId="6"/>
+    <tableColumn id="6" xr3:uid="{BF227374-82A0-4088-A70D-4967E9D58339}" name="Column6" headerRowDxfId="5" dataDxfId="4"/>
+    <tableColumn id="7" xr3:uid="{BA7D3376-9D4B-4B12-AB45-3526E423DA24}" name="Column7" headerRowDxfId="3" dataDxfId="2"/>
+    <tableColumn id="8" xr3:uid="{B23F41D5-4E64-4061-94AA-F7D64566A5B8}" name="Column8" headerRowDxfId="1" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium3" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1056,8 +2488,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J16" sqref="J16"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1566,31 +2998,31 @@
       <c r="A21" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="B21" s="4">
+      <c r="B21">
         <f>COUNT(Table6[Housing])</f>
         <v>12</v>
       </c>
-      <c r="C21" s="4">
+      <c r="C21">
         <f>COUNT(Table6[Bills &amp; Utilities])</f>
         <v>12</v>
       </c>
-      <c r="D21" s="4">
+      <c r="D21">
         <f>COUNT(Table6[Food &amp; Dining])</f>
         <v>12</v>
       </c>
-      <c r="E21" s="4">
+      <c r="E21">
         <f>COUNT(Table6[Personal])</f>
         <v>12</v>
       </c>
-      <c r="F21" s="4">
+      <c r="F21">
         <f>COUNT(Table6[Auto &amp; Transport])</f>
         <v>12</v>
       </c>
-      <c r="G21" s="4">
+      <c r="G21">
         <f>COUNT(Table6[Health &amp; Fitness])</f>
         <v>12</v>
       </c>
-      <c r="H21" s="4">
+      <c r="H21">
         <f>COUNT(Table6[Monthly Total])</f>
         <v>12</v>
       </c>
@@ -1635,4 +3067,137 @@
     <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{63898F7D-5B25-4E42-A07F-DB4F3B3FD3F2}">
+  <dimension ref="A3:B16"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="S8" sqref="S8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.44140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4" s="6">
+        <v>1695</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" s="6">
+        <v>1660</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" s="6">
+        <v>1650</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" s="6">
+        <v>1640</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B8" s="6">
+        <v>1650</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9" s="6">
+        <v>1650</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A10" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B10" s="6">
+        <v>1620</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A11" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B11" s="6">
+        <v>1650</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A12" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B12" s="6">
+        <v>1640</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A13" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B13" s="6">
+        <v>1670</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A14" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B14" s="6">
+        <v>1625</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A15" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B15" s="6">
+        <v>1670</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A16" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B16" s="6">
+        <v>19820</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>